<commit_message>
user friendly script added
</commit_message>
<xml_diff>
--- a/TestData/OneForAll/oneForAll.xlsx
+++ b/TestData/OneForAll/oneForAll.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pranav Pawar\PycharmProjects\RMM_DataDriven\TestData\OneForAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E96AC82-CE06-4705-B81C-956DBB7CA7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AF4B92-3AD1-4675-B29A-8296C46ACF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3708" yWindow="2700" windowWidth="18756" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="18756" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,39 +25,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Wave Name</t>
   </si>
   <si>
-    <t>Add New Wave</t>
-  </si>
-  <si>
-    <t>C:\Users\Pranav Pawar\PycharmProjects\RMM_DataDriven\TestData\OneForAll\createWaveWithHost1.xlsx</t>
-  </si>
-  <si>
-    <t>Passthrough</t>
-  </si>
-  <si>
-    <t>Add a Wave Without Host</t>
-  </si>
-  <si>
-    <t>Wave add by file</t>
-  </si>
-  <si>
     <t>Operation</t>
   </si>
   <si>
     <t>File Path Which Includes Data Related To Operation</t>
   </si>
   <si>
-    <t>First Wave 2</t>
-  </si>
-  <si>
-    <t>C:\Users\Pranav Pawar\PycharmProjects\RMM_DataDriven\TestData\OneForAll\First Flow 3.csv</t>
-  </si>
-  <si>
     <t>Host Name</t>
+  </si>
+  <si>
+    <t>Parallel Count</t>
+  </si>
+  <si>
+    <t>Policy Name</t>
+  </si>
+  <si>
+    <t>Row start from excel file</t>
+  </si>
+  <si>
+    <t>Row end from excel file</t>
+  </si>
+  <si>
+    <t>Datastore</t>
+  </si>
+  <si>
+    <t>Passthrough (True/False)</t>
+  </si>
+  <si>
+    <t>Test Mode (True/False)</t>
+  </si>
+  <si>
+    <t>Add wave with upload file</t>
+  </si>
+  <si>
+    <t>Add vCenter</t>
+  </si>
+  <si>
+    <t>C:\Users\Pranav Pawar\PycharmProjects\RMM_DataDriven\TestData\OneForAll\addVcenter.xlsx</t>
+  </si>
+  <si>
+    <t>Set Autoprovision</t>
+  </si>
+  <si>
+    <t>C:\Users\Pranav Pawar\PycharmProjects\RMM_DataDriven\TestData\OneForAll\setAutoprovisionAndNIC.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\Pranav Pawar\PycharmProjects\RMM_DataDriven\TestData\OneForAll\bulkEditOptions.xlsx</t>
+  </si>
+  <si>
+    <t>Edit Sync Options</t>
+  </si>
+  <si>
+    <t>C:\Users\Pranav Pawar\PycharmProjects\RMM_DataDriven\TestData\OneForAll\editSyncOptions.xlsx</t>
+  </si>
+  <si>
+    <t>Change Datastore for all waves</t>
+  </si>
+  <si>
+    <t>esx09-datastore2</t>
+  </si>
+  <si>
+    <t>Bulk Edit Sync options for wave</t>
+  </si>
+  <si>
+    <t>Bulk Edit Sync options for windows waves</t>
+  </si>
+  <si>
+    <t>C:\Users\Pranav Pawar\PycharmProjects\RMM_DataDriven\TestData\OneForAll\bulkEditOptionsWindows.xlsx</t>
+  </si>
+  <si>
+    <t>Set Parallel Count</t>
+  </si>
+  <si>
+    <t>Start wave and verify</t>
+  </si>
+  <si>
+    <t>Second Flow</t>
+  </si>
+  <si>
+    <t>C:\Users\Pranav Pawar\PycharmProjects\RMM_DataDriven\TestData\OneForAll\Second Flow.csv</t>
+  </si>
+  <si>
+    <t>Check Wave Status</t>
   </si>
 </sst>
 </file>
@@ -387,62 +441,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A2:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="91.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="K2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>